<commit_message>
projet presenté le 21/07/2020
</commit_message>
<xml_diff>
--- a/admin/files/Genie Logiciel.xlsx
+++ b/admin/files/Genie Logiciel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>MATRICULE</t>
   </si>
@@ -38,7 +38,10 @@
     <t>16TM445</t>
   </si>
   <si>
-    <t>16PK379</t>
+    <t>16PK389</t>
+  </si>
+  <si>
+    <t>²</t>
   </si>
 </sst>
 </file>
@@ -362,7 +365,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A8" sqref="A8:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -440,7 +443,9 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>

</xml_diff>